<commit_message>
almost ready for production we just have issue with the th it need to split
</commit_message>
<xml_diff>
--- a/result/INV PKL CT TH25008.xlsx
+++ b/result/INV PKL CT TH25008.xlsx
@@ -1443,7 +1443,7 @@
       </c>
       <c r="G3" s="133" t="inlineStr">
         <is>
-          <t>[[DATE]]</t>
+          <t>14/07/2025</t>
         </is>
       </c>
     </row>
@@ -1683,10 +1683,8 @@
       <c r="E20" s="37" t="n">
         <v>73409</v>
       </c>
-      <c r="F20" s="38" t="inlineStr">
-        <is>
-          <t>[[UNIT]]</t>
-        </is>
+      <c r="F20" s="38" t="n">
+        <v>1</v>
       </c>
       <c r="G20" s="38">
         <f>E20*F20</f>
@@ -2004,7 +2002,7 @@
       </c>
       <c r="G7" s="8" t="inlineStr">
         <is>
-          <t>[[REF]]</t>
+          <t>CLF2025-3</t>
         </is>
       </c>
     </row>
@@ -2050,7 +2048,7 @@
       </c>
       <c r="G9" s="16" t="inlineStr">
         <is>
-          <t>[[DATE]]</t>
+          <t>14/07/2025</t>
         </is>
       </c>
     </row>
@@ -2288,10 +2286,8 @@
       <c r="E22" s="37" t="n">
         <v>73409</v>
       </c>
-      <c r="F22" s="38" t="inlineStr">
-        <is>
-          <t>[[UNIT]]</t>
-        </is>
+      <c r="F22" s="38" t="n">
+        <v>1</v>
       </c>
       <c r="G22" s="38">
         <f>E22*F22</f>
@@ -2661,7 +2657,7 @@
       </c>
       <c r="I7" s="88" t="inlineStr">
         <is>
-          <t>[[REF]]</t>
+          <t>CLF2025-3</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2707,7 @@
       </c>
       <c r="I9" s="16" t="inlineStr">
         <is>
-          <t>[[DATE]]</t>
+          <t>14/07/2025</t>
         </is>
       </c>
     </row>

</xml_diff>